<commit_message>
added source osm to polygons
</commit_message>
<xml_diff>
--- a/Masterarbeit Plan.xlsx
+++ b/Masterarbeit Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Tag</t>
   </si>
@@ -441,6 +441,12 @@
   <si>
     <t>nützlicher code
 https://github.com/KaiserP/MasterThesis/blob/master/DownloadImages/berlin/code/download_city_data.py</t>
+  </si>
+  <si>
+    <t>1) Recherche: Aus openstreetmap polygone extrahieren</t>
+  </si>
+  <si>
+    <t>http://blog.rtwilson.com/how-to-convert-osm-waypoints-defining-polygons-into-shapefile/</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd/\ dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +560,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -583,11 +597,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -627,9 +642,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -911,8 +931,8 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,8 +1139,13 @@
         <v>43085</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="F14" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -2043,7 +2068,10 @@
       <c r="D121" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F14" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tried new polygon color method-fail
</commit_message>
<xml_diff>
--- a/Masterarbeit Plan.xlsx
+++ b/Masterarbeit Plan.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Tag</t>
   </si>
@@ -510,6 +511,41 @@
   <si>
     <t>Ideen für Straßenpolygone überlegen.
 Noch interessant: Wasser, Flüße, Seen, Bäume/Wald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4) Training und Evaluation implementieren mit TF/Keras/?? </t>
+  </si>
+  <si>
+    <t>  </t>
+  </si>
+  <si>
+    <t>   </t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Fertgestellt Am</t>
+  </si>
+  <si>
+    <t>Erhalten Am</t>
+  </si>
+  <si>
+    <t>Aufgabe</t>
+  </si>
+  <si>
+    <t>1) Daten sammeln,   
+Hast du da schon einen Crawler geschrieben,
+der automatisiert Daten von GMaps + OSM runterlädt?</t>
+  </si>
+  <si>
+    <t>2) Preprocessing    
+Weitere Klassen hinzufügen (außer Straßen) / Löcher in Polygonen füllen</t>
+  </si>
+  <si>
+    <t>3) Model  bauen
+Einfaches Segmentierungsmodell raussuchen (Paper Recherche!!) 
+und implementieren bzw. fertigs Modell verwenden</t>
   </si>
 </sst>
 </file>
@@ -519,7 +555,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd/\ dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,6 +675,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -694,7 +744,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -740,6 +790,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1026,9 +1087,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2193,4 +2254,409 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
+    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="67.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="48.75" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="19">
+        <v>43087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="22"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="23"/>
+      <c r="C5" s="21"/>
+    </row>
+    <row r="6" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="20"/>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="22"/>
+      <c r="C7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" ht="48.75" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="19">
+        <v>43087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="20"/>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="20"/>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="20"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="20"/>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="20"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="20"/>
+      <c r="C14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" ht="48.75" x14ac:dyDescent="0.35">
+      <c r="A15" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="19">
+        <v>43087</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="20"/>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="20"/>
+      <c r="C17" s="21"/>
+    </row>
+    <row r="18" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="C18" s="21"/>
+    </row>
+    <row r="19" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="C19" s="21"/>
+    </row>
+    <row r="20" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="C20" s="21"/>
+    </row>
+    <row r="21" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="19">
+        <v>43087</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C23" s="21"/>
+    </row>
+    <row r="24" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C24" s="21"/>
+    </row>
+    <row r="25" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C25" s="21"/>
+    </row>
+    <row r="26" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C26" s="21"/>
+    </row>
+    <row r="27" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C28" s="21"/>
+    </row>
+    <row r="29" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C32" s="21"/>
+    </row>
+    <row r="33" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C33" s="21"/>
+    </row>
+    <row r="34" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C34" s="21"/>
+    </row>
+    <row r="35" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C36" s="21"/>
+    </row>
+    <row r="37" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C37" s="21"/>
+    </row>
+    <row r="38" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C38" s="21"/>
+    </row>
+    <row r="39" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C39" s="21"/>
+    </row>
+    <row r="40" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C40" s="21"/>
+    </row>
+    <row r="41" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C41" s="21"/>
+    </row>
+    <row r="42" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C42" s="21"/>
+    </row>
+    <row r="43" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C44" s="21"/>
+    </row>
+    <row r="45" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C45" s="21"/>
+    </row>
+    <row r="46" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C46" s="21"/>
+    </row>
+    <row r="47" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C47" s="21"/>
+    </row>
+    <row r="48" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C48" s="21"/>
+    </row>
+    <row r="49" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C49" s="21"/>
+    </row>
+    <row r="50" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C50" s="21"/>
+    </row>
+    <row r="51" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C51" s="21"/>
+    </row>
+    <row r="52" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C52" s="21"/>
+    </row>
+    <row r="53" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C54" s="21"/>
+    </row>
+    <row r="55" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C55" s="21"/>
+    </row>
+    <row r="56" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C56" s="21"/>
+    </row>
+    <row r="57" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C57" s="21"/>
+    </row>
+    <row r="58" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C58" s="21"/>
+    </row>
+    <row r="59" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C59" s="21"/>
+    </row>
+    <row r="60" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C60" s="21"/>
+    </row>
+    <row r="61" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C61" s="21"/>
+    </row>
+    <row r="62" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C62" s="21"/>
+    </row>
+    <row r="63" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C63" s="21"/>
+    </row>
+    <row r="64" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C64" s="21"/>
+    </row>
+    <row r="65" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C65" s="21"/>
+    </row>
+    <row r="66" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C66" s="21"/>
+    </row>
+    <row r="67" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C67" s="21"/>
+    </row>
+    <row r="68" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C68" s="21"/>
+    </row>
+    <row r="69" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C69" s="21"/>
+    </row>
+    <row r="70" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C70" s="21"/>
+    </row>
+    <row r="71" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C71" s="21"/>
+    </row>
+    <row r="72" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C72" s="21"/>
+    </row>
+    <row r="73" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C73" s="21"/>
+    </row>
+    <row r="74" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C74" s="21"/>
+    </row>
+    <row r="75" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C75" s="21"/>
+    </row>
+    <row r="76" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C76" s="21"/>
+    </row>
+    <row r="77" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C77" s="21"/>
+    </row>
+    <row r="78" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C78" s="21"/>
+    </row>
+    <row r="79" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C79" s="21"/>
+    </row>
+    <row r="80" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C80" s="21"/>
+    </row>
+    <row r="81" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C81" s="21"/>
+    </row>
+    <row r="82" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C82" s="21"/>
+    </row>
+    <row r="83" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C83" s="21"/>
+    </row>
+    <row r="84" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C84" s="21"/>
+    </row>
+    <row r="85" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C85" s="21"/>
+    </row>
+    <row r="86" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C86" s="21"/>
+    </row>
+    <row r="87" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C87" s="21"/>
+    </row>
+    <row r="88" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C88" s="21"/>
+    </row>
+    <row r="89" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C89" s="21"/>
+    </row>
+    <row r="90" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C90" s="21"/>
+    </row>
+    <row r="91" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C91" s="21"/>
+    </row>
+    <row r="92" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C92" s="21"/>
+    </row>
+    <row r="93" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C93" s="21"/>
+    </row>
+    <row r="94" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C94" s="21"/>
+    </row>
+    <row r="95" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C95" s="21"/>
+    </row>
+    <row r="96" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C96" s="21"/>
+    </row>
+    <row r="97" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C97" s="21"/>
+    </row>
+    <row r="98" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C98" s="21"/>
+    </row>
+    <row r="99" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C99" s="21"/>
+    </row>
+    <row r="100" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C100" s="21"/>
+    </row>
+    <row r="101" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C101" s="21"/>
+    </row>
+    <row r="102" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C102" s="21"/>
+    </row>
+    <row r="103" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C103" s="21"/>
+    </row>
+    <row r="104" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C104" s="21"/>
+    </row>
+    <row r="105" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C105" s="21"/>
+    </row>
+    <row r="106" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C106" s="21"/>
+    </row>
+    <row r="107" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C107" s="21"/>
+    </row>
+    <row r="108" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C108" s="21"/>
+    </row>
+    <row r="109" spans="3:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C109" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added zoom example (potential fix for diff zoom in osm gmaps)
</commit_message>
<xml_diff>
--- a/Masterarbeit Plan.xlsx
+++ b/Masterarbeit Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -10,7 +10,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Tag</t>
   </si>
@@ -551,11 +551,17 @@
     <t>Problem: Zoom levels stimmen offensichtlich
  nicht überein bei osm und googlemaps</t>
   </si>
+  <si>
+    <t>https://stackoverflow.com/a/37121993/8862202</t>
+  </si>
+  <si>
+    <t>Zoom googlemap pngs damit sie das gleiche zeigen wie osm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd/\ dd/mm/yyyy"/>
   </numFmts>
@@ -1091,9 +1097,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1363,12 @@
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -2254,9 +2265,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F14" r:id="rId1"/>
+    <hyperlink ref="E17" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Idea 2 implementation + schedule upd
</commit_message>
<xml_diff>
--- a/Masterarbeit Plan.xlsx
+++ b/Masterarbeit Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Tag</t>
   </si>
@@ -574,15 +574,34 @@
     <t>Quelle für Idee 1 (Zoom):
 https://stackoverflow.com/a/37121993/8862202
 Idee 2:
-(Berechne Bbox von gmaps image):
-https://gis.stackexchange.com/questions/46729/corner-coordinates-of-google-static-map-tile
-(Laden von OSM mit bbox): http://wiki.openstreetmap.org/wiki/Downloading_data</t>
+Lade Bild aus google-Maps(mit zoom, long, lat). Berechne BoundingBox dieses Bildes. Dann lade Osm mit der gleichen Boundingbox herunter.</t>
+  </si>
+  <si>
+    <t>Vortrag über Skynet: (Der Kerl hat nicht so Ahnung)
+https://2016.stateofthemap.us/skynet/</t>
+  </si>
+  <si>
+    <t>Proposal angefangen</t>
   </si>
   <si>
     <t>Quelle für Idee 1 (Zoom):
 https://stackoverflow.com/a/37121993/8862202
 Idee 2:
-Lade Bild aus google-Maps(mit zoom, long, lat). Berechne BoundingBox dieses Bildes. Dann lade Osm mit der gleichen Boundingbox herunter.</t>
+(Berechne Bbox von gmaps image):
+https://gis.stackexchange.com/questions/46729/corner-coordinates-of-google-static-map-tile
+(Laden von OSM mit bbox): http://wiki.openstreetmap.org/wiki/Downloading_data
+http://api.openstreetmap.org/api/0.6/map?bbox=11.54,48.14,11.543,48.145</t>
+  </si>
+  <si>
+    <t>Implementierung Idee 2:
+BoundingBox von gegebenem Google Satelliten-Bild bestimmen</t>
+  </si>
+  <si>
+    <t>Input: zoom, lat, long, width, height
+Output: left, bottom, right, top</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/12507274/how-to-get-bounds-of-a-google-static-map</t>
   </si>
 </sst>
 </file>
@@ -790,7 +809,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -851,6 +870,10 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Ausgabe" xfId="3" builtinId="21"/>
@@ -1137,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
@@ -1403,7 +1426,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43088</v>
       </c>
@@ -1417,7 +1440,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1464,21 +1487,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43094</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="9">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E23" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43095</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="2"/>
+      <c r="B24" s="9">
+        <v>3</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -1521,7 +1560,7 @@
       <c r="D29" s="2"/>
       <c r="G29">
         <f t="shared" ref="G29" si="2">SUM(B23:B29)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2325,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2371,7 +2410,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="21"/>
     </row>

</xml_diff>